<commit_message>
Add some observations to the results
Signed-off-by: Henrique V. Ehrenfried <hvehrenfried@inf.ufpr.br>
</commit_message>
<xml_diff>
--- a/Comparisons/all_results.xlsx
+++ b/Comparisons/all_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hvehr\Documents\Doutorado\AnalysisResultsTextGCN\Comparisons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{472420D2-5844-40C1-A03F-5EAF66473992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8CB368-0E9A-45DC-BDD0-BB6C1E6016B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="all_results" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="53">
   <si>
     <t>Dataset</t>
   </si>
@@ -155,6 +154,36 @@
   </si>
   <si>
     <t>R52</t>
+  </si>
+  <si>
+    <t>Quanto maior o Early Stopping, menor a acurácia. Provavelmente esteja acontecendo overfitting</t>
+  </si>
+  <si>
+    <t>Quanto menor o Learning Rate, melhor o resultado</t>
+  </si>
+  <si>
+    <t>Quanto maior o Dropout, melhor o resultado</t>
+  </si>
+  <si>
+    <t>Hidden 1 não parece afetar o resultado</t>
+  </si>
+  <si>
+    <t>Quanto menor o Dropout, melhor o resultado</t>
+  </si>
+  <si>
+    <t>Learning Rate não pode ser muito baixo, nem muito alto porque pode afetar o resultado</t>
+  </si>
+  <si>
+    <t>Dropout não influencia muito o resultado deste conjunto de dados</t>
+  </si>
+  <si>
+    <t>Early stopping mais alto é melhor para esse dataset, logo ele não gera overfitting com tanta facilidade</t>
+  </si>
+  <si>
+    <t>Hidden 1 parece ter algum impacto sobre esse dataset</t>
+  </si>
+  <si>
+    <t>Dropout parece ter algum impacto sobre esse dataset</t>
   </si>
 </sst>
 </file>
@@ -237,7 +266,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -292,13 +321,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -307,65 +336,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -407,6 +378,114 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -416,167 +495,111 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good_results" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF008E40"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF00823B"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <b/>
@@ -644,56 +667,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF00823B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF008E40"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF00823B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1093,13 +1066,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O78"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -1116,9 +1089,10 @@
     <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="31" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="55.42578125" style="59" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1165,8 +1139,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="4">
@@ -1208,12 +1182,15 @@
       <c r="N2" s="4">
         <v>-8.0999999999999996E-3</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="55" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="39"/>
+      <c r="P2" s="60" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="33"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -1253,12 +1230,13 @@
       <c r="N3" s="2">
         <v>-4.3900000000000002E-2</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="39"/>
+      <c r="O3" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="61"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="33"/>
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -1298,12 +1276,13 @@
       <c r="N4" s="2">
         <v>-5.6399999999999999E-2</v>
       </c>
-      <c r="O4" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="39"/>
+      <c r="O4" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="61"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="33"/>
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -1343,12 +1322,15 @@
       <c r="N5" s="2">
         <v>-1.5100000000000001E-2</v>
       </c>
-      <c r="O5" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="39"/>
+      <c r="O5" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="33"/>
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -1388,12 +1370,13 @@
       <c r="N6" s="2">
         <v>-8.2000000000000007E-3</v>
       </c>
-      <c r="O6" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
+      <c r="O6" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" s="61"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="33"/>
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -1433,12 +1416,13 @@
       <c r="N7" s="2">
         <v>-7.1999999999999998E-3</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="O7" s="56" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="39"/>
+      <c r="P7" s="61"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="33"/>
       <c r="B8" s="2">
         <v>6</v>
       </c>
@@ -1478,12 +1462,13 @@
       <c r="N8" s="2">
         <v>-6.7999999999999996E-3</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="O8" s="56" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="39"/>
+      <c r="P8" s="61"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="33"/>
       <c r="B9" s="2">
         <v>7</v>
       </c>
@@ -1523,12 +1508,15 @@
       <c r="N9" s="2">
         <v>-1.09E-2</v>
       </c>
-      <c r="O9" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="39"/>
+      <c r="O9" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" s="61" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="33"/>
       <c r="B10" s="2">
         <v>8</v>
       </c>
@@ -1568,12 +1556,13 @@
       <c r="N10" s="2">
         <v>-1.01E-2</v>
       </c>
-      <c r="O10" s="7" t="s">
+      <c r="O10" s="56" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="39"/>
+      <c r="P10" s="61"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="33"/>
       <c r="B11" s="2">
         <v>9</v>
       </c>
@@ -1613,12 +1602,13 @@
       <c r="N11" s="2">
         <v>-9.2999999999999992E-3</v>
       </c>
-      <c r="O11" s="7" t="s">
+      <c r="O11" s="56" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="39"/>
+      <c r="P11" s="61"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="33"/>
       <c r="B12" s="2">
         <v>10</v>
       </c>
@@ -1658,12 +1648,13 @@
       <c r="N12" s="2">
         <v>-8.8000000000000005E-3</v>
       </c>
-      <c r="O12" s="7" t="s">
+      <c r="O12" s="56" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="39"/>
+      <c r="P12" s="61"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="33"/>
       <c r="B13" s="2">
         <v>11</v>
       </c>
@@ -1703,12 +1694,13 @@
       <c r="N13" s="2">
         <v>-8.3999999999999995E-3</v>
       </c>
-      <c r="O13" s="7" t="s">
+      <c r="O13" s="56" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="39"/>
+      <c r="P13" s="61"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="33"/>
       <c r="B14" s="2">
         <v>12</v>
       </c>
@@ -1748,12 +1740,13 @@
       <c r="N14" s="2">
         <v>-7.9000000000000008E-3</v>
       </c>
-      <c r="O14" s="7" t="s">
+      <c r="O14" s="56" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
+      <c r="P14" s="61"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="33"/>
       <c r="B15" s="2">
         <v>13</v>
       </c>
@@ -1793,57 +1786,59 @@
       <c r="N15" s="2">
         <v>-7.1000000000000004E-3</v>
       </c>
-      <c r="O15" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="39"/>
-      <c r="B16" s="56">
+      <c r="O15" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="P15" s="61"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="33"/>
+      <c r="B16" s="30">
         <v>14</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="56">
+      <c r="D16" s="30">
         <v>0.76119999999999999</v>
       </c>
-      <c r="E16" s="56">
+      <c r="E16" s="30">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="F16" s="56">
+      <c r="F16" s="30">
         <v>0.76739999999999997</v>
       </c>
-      <c r="G16" s="56">
+      <c r="G16" s="30">
         <v>2E-3</v>
       </c>
-      <c r="H16" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="56">
-        <v>0.03</v>
-      </c>
-      <c r="J16" s="56">
+      <c r="H16" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="30">
+        <v>0.03</v>
+      </c>
+      <c r="J16" s="30">
         <v>8.8244000000000007</v>
       </c>
-      <c r="K16" s="56">
+      <c r="K16" s="30">
         <v>0</v>
       </c>
-      <c r="L16" s="56">
+      <c r="L16" s="30">
         <v>99.999899999999997</v>
       </c>
-      <c r="M16" s="56" t="s">
+      <c r="M16" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="N16" s="56">
+      <c r="N16" s="30">
         <v>-6.1999999999999998E-3</v>
       </c>
-      <c r="O16" s="58" t="s">
+      <c r="O16" s="57" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="39"/>
+      <c r="P16" s="61"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="33"/>
       <c r="B17" s="2">
         <v>15</v>
       </c>
@@ -1883,12 +1878,13 @@
       <c r="N17" s="2">
         <v>-6.1999999999999998E-3</v>
       </c>
-      <c r="O17" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="39"/>
+      <c r="O17" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="P17" s="61"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="33"/>
       <c r="B18" s="2">
         <v>16</v>
       </c>
@@ -1928,12 +1924,15 @@
       <c r="N18" s="2">
         <v>-8.0999999999999996E-3</v>
       </c>
-      <c r="O18" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="39"/>
+      <c r="O18" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18" s="61" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="33"/>
       <c r="B19" s="2">
         <v>17</v>
       </c>
@@ -1973,2660 +1972,2758 @@
       <c r="N19" s="2">
         <v>-8.6E-3</v>
       </c>
-      <c r="O19" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
-      <c r="B20" s="8">
+      <c r="O19" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" s="61"/>
+    </row>
+    <row r="20" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
+      <c r="B20" s="6">
         <v>18</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="6">
         <v>0.75890000000000002</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="6">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="6">
         <v>0.76739999999999997</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="6">
         <v>2E-3</v>
       </c>
-      <c r="H20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="8">
-        <v>0.03</v>
-      </c>
-      <c r="J20" s="8">
+      <c r="H20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="J20" s="6">
         <v>11.9216</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20" s="6">
         <v>0</v>
       </c>
-      <c r="L20" s="8">
+      <c r="L20" s="6">
         <v>100</v>
       </c>
-      <c r="M20" s="8" t="s">
+      <c r="M20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N20" s="8">
+      <c r="N20" s="6">
         <v>-8.5000000000000006E-3</v>
       </c>
-      <c r="O20" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="41" t="s">
+      <c r="O20" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="P20" s="62"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="10">
         <v>0</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="10">
         <v>0.68689999999999996</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="10">
         <v>3.3E-3</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="10">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="10">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="H21" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I21" s="13">
-        <v>0.03</v>
-      </c>
-      <c r="J21" s="13">
+      <c r="I21" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="J21" s="10">
         <v>-1.6302000000000001</v>
       </c>
-      <c r="K21" s="13">
+      <c r="K21" s="10">
         <v>0.12039999999999999</v>
       </c>
-      <c r="L21" s="13">
+      <c r="L21" s="10">
         <v>87.956999999999994</v>
       </c>
-      <c r="M21" s="13" t="s">
+      <c r="M21" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="N21" s="13">
+      <c r="N21" s="10">
         <v>3.3E-3</v>
       </c>
-      <c r="O21" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
-      <c r="B22" s="11">
+      <c r="O21" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="P21" s="60" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="36"/>
+      <c r="B22" s="8">
         <v>1</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="8">
         <v>0.68620000000000003</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="8">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="H22" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I22" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J22" s="11">
+      <c r="I22" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J22" s="8">
         <v>-1.3936999999999999</v>
       </c>
-      <c r="K22" s="11">
+      <c r="K22" s="8">
         <v>0.18940000000000001</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="8">
         <v>81.058599999999998</v>
       </c>
-      <c r="M22" s="11" t="s">
+      <c r="M22" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N22" s="11">
+      <c r="N22" s="8">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="O22" s="16" t="s">
+      <c r="O22" s="52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
-      <c r="B23" s="11">
+      <c r="P22" s="61"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="36"/>
+      <c r="B23" s="8">
         <v>2</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="8">
         <v>0.67130000000000001</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="8">
         <v>1.4E-3</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H23" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J23" s="11">
+      <c r="H23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J23" s="8">
         <v>6.7107000000000001</v>
       </c>
-      <c r="K23" s="11">
+      <c r="K23" s="8">
         <v>0</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="8">
         <v>99.995099999999994</v>
       </c>
-      <c r="M23" s="11" t="s">
+      <c r="M23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N23" s="8">
         <v>-1.23E-2</v>
       </c>
-      <c r="O23" s="16" t="s">
+      <c r="O23" s="52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
-      <c r="B24" s="11">
+      <c r="P23" s="61"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="36"/>
+      <c r="B24" s="8">
         <v>3</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="8">
         <v>0.67820000000000003</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="8">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H24" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J24" s="11">
+      <c r="H24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J24" s="8">
         <v>2.3664999999999998</v>
       </c>
-      <c r="K24" s="11">
+      <c r="K24" s="8">
         <v>2.9399999999999999E-2</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="8">
         <v>97.062299999999993</v>
       </c>
-      <c r="M24" s="11" t="s">
+      <c r="M24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N24" s="11">
+      <c r="N24" s="8">
         <v>-5.4000000000000003E-3</v>
       </c>
-      <c r="O24" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
-      <c r="B25" s="11">
+      <c r="O24" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="P24" s="61" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="36"/>
+      <c r="B25" s="8">
         <v>4</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="8">
         <v>0.68640000000000001</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="8">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H25" s="12" t="s">
+      <c r="H25" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I25" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J25" s="11">
+      <c r="I25" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J25" s="8">
         <v>-1.3541000000000001</v>
       </c>
-      <c r="K25" s="11">
+      <c r="K25" s="8">
         <v>0.1925</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="8">
         <v>80.754900000000006</v>
       </c>
-      <c r="M25" s="11" t="s">
+      <c r="M25" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N25" s="11">
+      <c r="N25" s="8">
         <v>2.8E-3</v>
       </c>
-      <c r="O25" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="42"/>
-      <c r="B26" s="11">
+      <c r="O25" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="P25" s="61"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="36"/>
+      <c r="B26" s="8">
         <v>5</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="8">
         <v>0.67659999999999998</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="8">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H26" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J26" s="11">
+      <c r="H26" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J26" s="8">
         <v>3.7591000000000001</v>
       </c>
-      <c r="K26" s="11">
+      <c r="K26" s="8">
         <v>3.3E-3</v>
       </c>
-      <c r="L26" s="11">
+      <c r="L26" s="8">
         <v>99.670699999999997</v>
       </c>
-      <c r="M26" s="11" t="s">
+      <c r="M26" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N26" s="11">
+      <c r="N26" s="8">
         <v>-7.0000000000000001E-3</v>
       </c>
-      <c r="O26" s="16" t="s">
+      <c r="O26" s="52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
-      <c r="B27" s="11">
+      <c r="P26" s="61"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="36"/>
+      <c r="B27" s="8">
         <v>6</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="8">
         <v>0.67100000000000004</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="8">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H27" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J27" s="11">
+      <c r="H27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J27" s="8">
         <v>6.4661999999999997</v>
       </c>
-      <c r="K27" s="11">
+      <c r="K27" s="8">
         <v>0</v>
       </c>
-      <c r="L27" s="11">
+      <c r="L27" s="8">
         <v>99.997500000000002</v>
       </c>
-      <c r="M27" s="11" t="s">
+      <c r="M27" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N27" s="11">
+      <c r="N27" s="8">
         <v>-1.26E-2</v>
       </c>
-      <c r="O27" s="16" t="s">
+      <c r="O27" s="52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="42"/>
-      <c r="B28" s="53">
+      <c r="P27" s="61"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="36"/>
+      <c r="B28" s="28">
         <v>7</v>
       </c>
-      <c r="C28" s="53" t="s">
+      <c r="C28" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="53">
+      <c r="D28" s="28">
         <v>0.68859999999999999</v>
       </c>
-      <c r="E28" s="53">
+      <c r="E28" s="28">
         <v>1.8E-3</v>
       </c>
-      <c r="F28" s="53">
+      <c r="F28" s="28">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G28" s="53">
+      <c r="G28" s="28">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H28" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="53">
-        <v>0.03</v>
-      </c>
-      <c r="J28" s="53">
+      <c r="H28" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="28">
+        <v>0.03</v>
+      </c>
+      <c r="J28" s="28">
         <v>-2.6920000000000002</v>
       </c>
-      <c r="K28" s="53">
+      <c r="K28" s="28">
         <v>2.1299999999999999E-2</v>
       </c>
-      <c r="L28" s="53">
+      <c r="L28" s="28">
         <v>97.868899999999996</v>
       </c>
-      <c r="M28" s="53" t="s">
+      <c r="M28" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="N28" s="53">
+      <c r="N28" s="28">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="O28" s="55" t="s">
+      <c r="O28" s="53" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="42"/>
-      <c r="B29" s="11">
+      <c r="P28" s="61" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="36"/>
+      <c r="B29" s="8">
         <v>8</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="8">
         <v>0.68789999999999996</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="8">
         <v>1.9E-3</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H29" s="12" t="s">
+      <c r="H29" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J29" s="11">
+      <c r="I29" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J29" s="8">
         <v>-2.3182999999999998</v>
       </c>
-      <c r="K29" s="11">
+      <c r="K29" s="8">
         <v>4.07E-2</v>
       </c>
-      <c r="L29" s="11">
+      <c r="L29" s="8">
         <v>95.929599999999994</v>
       </c>
-      <c r="M29" s="11" t="s">
+      <c r="M29" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N29" s="11">
+      <c r="N29" s="8">
         <v>4.3E-3</v>
       </c>
-      <c r="O29" s="16" t="s">
+      <c r="O29" s="52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="42"/>
-      <c r="B30" s="11">
+      <c r="P29" s="61"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="36"/>
+      <c r="B30" s="8">
         <v>9</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="8">
         <v>0.68840000000000001</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="8">
         <v>1.5E-3</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H30" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J30" s="11">
+      <c r="H30" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J30" s="8">
         <v>-2.6072000000000002</v>
       </c>
-      <c r="K30" s="11">
+      <c r="K30" s="8">
         <v>2.5700000000000001E-2</v>
       </c>
-      <c r="L30" s="11">
+      <c r="L30" s="8">
         <v>97.431100000000001</v>
       </c>
-      <c r="M30" s="11" t="s">
+      <c r="M30" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N30" s="11">
+      <c r="N30" s="8">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="O30" s="16" t="s">
+      <c r="O30" s="52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="42"/>
-      <c r="B31" s="11">
+      <c r="P30" s="61"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="36"/>
+      <c r="B31" s="8">
         <v>10</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="8">
         <v>0.68740000000000001</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="8">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="H31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I31" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J31" s="11">
+      <c r="I31" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J31" s="8">
         <v>-2.0897999999999999</v>
       </c>
-      <c r="K31" s="11">
+      <c r="K31" s="8">
         <v>6.3700000000000007E-2</v>
       </c>
-      <c r="L31" s="11">
+      <c r="L31" s="8">
         <v>93.634100000000004</v>
       </c>
-      <c r="M31" s="11" t="s">
+      <c r="M31" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N31" s="11">
+      <c r="N31" s="8">
         <v>3.8E-3</v>
       </c>
-      <c r="O31" s="16" t="s">
+      <c r="O31" s="52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="42"/>
-      <c r="B32" s="11">
+      <c r="P31" s="61"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" s="36"/>
+      <c r="B32" s="8">
         <v>11</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="8">
         <v>0.68659999999999999</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="8">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H32" s="12" t="s">
+      <c r="H32" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I32" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J32" s="11">
+      <c r="I32" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J32" s="8">
         <v>-1.6237999999999999</v>
       </c>
-      <c r="K32" s="11">
+      <c r="K32" s="8">
         <v>0.13400000000000001</v>
       </c>
-      <c r="L32" s="11">
+      <c r="L32" s="8">
         <v>86.598799999999997</v>
       </c>
-      <c r="M32" s="11" t="s">
+      <c r="M32" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N32" s="11">
+      <c r="N32" s="8">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="O32" s="16" t="s">
+      <c r="O32" s="52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="42"/>
-      <c r="B33" s="11">
+      <c r="P32" s="61"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" s="36"/>
+      <c r="B33" s="8">
         <v>12</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="8">
         <v>0.68530000000000002</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="8">
         <v>1.9E-3</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H33" s="12" t="s">
+      <c r="H33" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I33" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J33" s="11">
+      <c r="I33" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J33" s="8">
         <v>-0.88770000000000004</v>
       </c>
-      <c r="K33" s="11">
+      <c r="K33" s="8">
         <v>0.39369999999999999</v>
       </c>
-      <c r="L33" s="11">
+      <c r="L33" s="8">
         <v>60.634799999999998</v>
       </c>
-      <c r="M33" s="11" t="s">
+      <c r="M33" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N33" s="11">
+      <c r="N33" s="8">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="O33" s="16" t="s">
+      <c r="O33" s="52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="42"/>
-      <c r="B34" s="11">
+      <c r="P33" s="61"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" s="36"/>
+      <c r="B34" s="8">
         <v>13</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="8">
         <v>0.68620000000000003</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E34" s="8">
         <v>2.8E-3</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F34" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H34" s="12" t="s">
+      <c r="H34" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I34" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J34" s="11">
+      <c r="I34" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J34" s="8">
         <v>-1.2986</v>
       </c>
-      <c r="K34" s="11">
+      <c r="K34" s="8">
         <v>0.21049999999999999</v>
       </c>
-      <c r="L34" s="11">
+      <c r="L34" s="8">
         <v>78.952200000000005</v>
       </c>
-      <c r="M34" s="11" t="s">
+      <c r="M34" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N34" s="11">
+      <c r="N34" s="8">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="O34" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
-      <c r="B35" s="11">
+      <c r="O34" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="P34" s="61"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" s="36"/>
+      <c r="B35" s="8">
         <v>14</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="8">
         <v>0.68410000000000004</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E35" s="8">
         <v>3.0999999999999999E-3</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F35" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G35" s="11">
+      <c r="G35" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H35" s="12" t="s">
+      <c r="H35" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I35" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J35" s="11">
+      <c r="I35" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J35" s="8">
         <v>-0.25659999999999999</v>
       </c>
-      <c r="K35" s="11">
+      <c r="K35" s="8">
         <v>0.8004</v>
       </c>
-      <c r="L35" s="11">
+      <c r="L35" s="8">
         <v>19.9635</v>
       </c>
-      <c r="M35" s="11" t="s">
+      <c r="M35" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N35" s="11">
+      <c r="N35" s="8">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O35" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="42"/>
-      <c r="B36" s="11">
+      <c r="O35" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="P35" s="61"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" s="36"/>
+      <c r="B36" s="8">
         <v>15</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="8">
         <v>0.68200000000000005</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E36" s="8">
         <v>3.3E-3</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G36" s="11">
+      <c r="G36" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H36" s="12" t="s">
+      <c r="H36" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I36" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J36" s="11">
+      <c r="I36" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J36" s="8">
         <v>0.79530000000000001</v>
       </c>
-      <c r="K36" s="11">
+      <c r="K36" s="8">
         <v>0.43680000000000002</v>
       </c>
-      <c r="L36" s="11">
+      <c r="L36" s="8">
         <v>56.320099999999996</v>
       </c>
-      <c r="M36" s="11" t="s">
+      <c r="M36" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N36" s="11">
+      <c r="N36" s="8">
         <v>-1.6000000000000001E-3</v>
       </c>
-      <c r="O36" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="42"/>
-      <c r="B37" s="11">
+      <c r="O36" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="P36" s="61"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" s="36"/>
+      <c r="B37" s="8">
         <v>16</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="11">
+      <c r="D37" s="8">
         <v>0.67869999999999997</v>
       </c>
-      <c r="E37" s="11">
+      <c r="E37" s="8">
         <v>1.9E-3</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F37" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G37" s="11">
+      <c r="G37" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H37" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I37" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J37" s="11">
+      <c r="H37" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J37" s="8">
         <v>2.6391</v>
       </c>
-      <c r="K37" s="11">
+      <c r="K37" s="8">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="L37" s="11">
+      <c r="L37" s="8">
         <v>97.715900000000005</v>
       </c>
-      <c r="M37" s="11" t="s">
+      <c r="M37" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N37" s="11">
+      <c r="N37" s="8">
         <v>-4.8999999999999998E-3</v>
       </c>
-      <c r="O37" s="16" t="s">
+      <c r="O37" s="52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="42"/>
-      <c r="B38" s="11">
-        <v>17</v>
-      </c>
-      <c r="C38" s="11" t="s">
+      <c r="P37" s="61" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" s="36"/>
+      <c r="B38" s="8">
+        <v>17</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="8">
         <v>0.6875</v>
       </c>
-      <c r="E38" s="11">
+      <c r="E38" s="8">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="F38" s="11">
+      <c r="F38" s="8">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G38" s="11">
+      <c r="G38" s="8">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H38" s="12" t="s">
+      <c r="H38" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I38" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="J38" s="11">
+      <c r="I38" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J38" s="8">
         <v>-2.0375000000000001</v>
       </c>
-      <c r="K38" s="11">
+      <c r="K38" s="8">
         <v>6.5199999999999994E-2</v>
       </c>
-      <c r="L38" s="11">
+      <c r="L38" s="8">
         <v>93.477599999999995</v>
       </c>
-      <c r="M38" s="11" t="s">
+      <c r="M38" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N38" s="11">
+      <c r="N38" s="8">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="O38" s="16" t="s">
+      <c r="O38" s="52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
-      <c r="B39" s="17">
+      <c r="P38" s="61"/>
+    </row>
+    <row r="39" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="37"/>
+      <c r="B39" s="12">
         <v>18</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="12">
         <v>0.68799999999999994</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="12">
         <v>1.8E-3</v>
       </c>
-      <c r="F39" s="17">
+      <c r="F39" s="12">
         <v>0.68359999999999999</v>
       </c>
-      <c r="G39" s="17">
+      <c r="G39" s="12">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="H39" s="18" t="s">
+      <c r="H39" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="I39" s="17">
-        <v>0.03</v>
-      </c>
-      <c r="J39" s="17">
+      <c r="I39" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="J39" s="12">
         <v>-2.3792</v>
       </c>
-      <c r="K39" s="17">
+      <c r="K39" s="12">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="L39" s="17">
+      <c r="L39" s="12">
         <v>96.319500000000005</v>
       </c>
-      <c r="M39" s="17" t="s">
+      <c r="M39" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="N39" s="17">
+      <c r="N39" s="12">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="O39" s="19" t="s">
+      <c r="O39" s="54" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="44" t="s">
+      <c r="P39" s="62"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="22">
+      <c r="B40" s="16">
         <v>0</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="16">
         <v>0.97160000000000002</v>
       </c>
-      <c r="E40" s="22">
+      <c r="E40" s="16">
         <v>1.5E-3</v>
       </c>
-      <c r="F40" s="22">
+      <c r="F40" s="16">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G40" s="22">
+      <c r="G40" s="16">
         <v>1E-3</v>
       </c>
-      <c r="H40" s="23" t="s">
+      <c r="H40" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I40" s="22">
-        <v>0.03</v>
-      </c>
-      <c r="J40" s="22">
+      <c r="I40" s="16">
+        <v>0.03</v>
+      </c>
+      <c r="J40" s="16">
         <v>-1.6574</v>
       </c>
-      <c r="K40" s="22">
+      <c r="K40" s="16">
         <v>0.1148</v>
       </c>
-      <c r="L40" s="22">
+      <c r="L40" s="16">
         <v>88.523399999999995</v>
       </c>
-      <c r="M40" s="22" t="s">
+      <c r="M40" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="N40" s="22">
+      <c r="N40" s="16">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="O40" s="24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="45"/>
-      <c r="B41" s="20">
+      <c r="O40" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="P40" s="60" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" s="39"/>
+      <c r="B41" s="14">
         <v>1</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="20">
+      <c r="D41" s="14">
         <v>0.96940000000000004</v>
       </c>
-      <c r="E41" s="20">
+      <c r="E41" s="14">
         <v>1E-3</v>
       </c>
-      <c r="F41" s="20">
+      <c r="F41" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G41" s="20">
+      <c r="G41" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H41" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I41" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J41" s="20">
+      <c r="H41" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J41" s="14">
         <v>2.8952</v>
       </c>
-      <c r="K41" s="20">
+      <c r="K41" s="14">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="L41" s="20">
+      <c r="L41" s="14">
         <v>99.035399999999996</v>
       </c>
-      <c r="M41" s="20" t="s">
+      <c r="M41" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="N41" s="20">
+      <c r="N41" s="14">
         <v>-1.2999999999999999E-3</v>
       </c>
-      <c r="O41" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="45"/>
-      <c r="B42" s="20">
+      <c r="O41" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P41" s="61"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" s="39"/>
+      <c r="B42" s="14">
         <v>2</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="20">
+      <c r="D42" s="14">
         <v>0.96619999999999995</v>
       </c>
-      <c r="E42" s="20">
+      <c r="E42" s="14">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="F42" s="20">
+      <c r="F42" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G42" s="20">
+      <c r="G42" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H42" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I42" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J42" s="20">
+      <c r="H42" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I42" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J42" s="14">
         <v>9.5426000000000002</v>
       </c>
-      <c r="K42" s="20">
+      <c r="K42" s="14">
         <v>0</v>
       </c>
-      <c r="L42" s="20">
+      <c r="L42" s="14">
         <v>100</v>
       </c>
-      <c r="M42" s="20" t="s">
+      <c r="M42" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="N42" s="20">
+      <c r="N42" s="14">
         <v>-4.4999999999999997E-3</v>
       </c>
-      <c r="O42" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="45"/>
-      <c r="B43" s="20">
+      <c r="O42" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P42" s="61"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" s="39"/>
+      <c r="B43" s="14">
         <v>3</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="20">
+      <c r="D43" s="14">
         <v>0.96499999999999997</v>
       </c>
-      <c r="E43" s="20">
+      <c r="E43" s="14">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="F43" s="20">
+      <c r="F43" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G43" s="20">
+      <c r="G43" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H43" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I43" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J43" s="20">
+      <c r="H43" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J43" s="14">
         <v>9.5767000000000007</v>
       </c>
-      <c r="K43" s="20">
+      <c r="K43" s="14">
         <v>0</v>
       </c>
-      <c r="L43" s="20">
+      <c r="L43" s="14">
         <v>100</v>
       </c>
-      <c r="M43" s="20" t="s">
+      <c r="M43" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="N43" s="20">
+      <c r="N43" s="14">
         <v>-5.7000000000000002E-3</v>
       </c>
-      <c r="O43" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="45"/>
-      <c r="B44" s="50">
+      <c r="O43" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P43" s="61" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" s="39"/>
+      <c r="B44" s="26">
         <v>4</v>
       </c>
-      <c r="C44" s="50" t="s">
+      <c r="C44" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="50">
+      <c r="D44" s="26">
         <v>0.97360000000000002</v>
       </c>
-      <c r="E44" s="50">
+      <c r="E44" s="26">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="F44" s="50">
+      <c r="F44" s="26">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G44" s="50">
+      <c r="G44" s="26">
         <v>1E-3</v>
       </c>
-      <c r="H44" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="I44" s="50">
-        <v>0.03</v>
-      </c>
-      <c r="J44" s="50">
+      <c r="H44" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I44" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="J44" s="26">
         <v>-7.4744999999999999</v>
       </c>
-      <c r="K44" s="50">
+      <c r="K44" s="26">
         <v>0</v>
       </c>
-      <c r="L44" s="50">
+      <c r="L44" s="26">
         <v>99.999899999999997</v>
       </c>
-      <c r="M44" s="50" t="s">
+      <c r="M44" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="N44" s="50">
+      <c r="N44" s="26">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="O44" s="52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="45"/>
-      <c r="B45" s="20">
+      <c r="O44" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="P44" s="61"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" s="39"/>
+      <c r="B45" s="14">
         <v>5</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C45" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="20">
+      <c r="D45" s="14">
         <v>0.97119999999999995</v>
       </c>
-      <c r="E45" s="20">
+      <c r="E45" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="F45" s="20">
+      <c r="F45" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G45" s="20">
+      <c r="G45" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H45" s="21" t="s">
+      <c r="H45" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I45" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J45" s="20">
+      <c r="I45" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J45" s="14">
         <v>-1.3293999999999999</v>
       </c>
-      <c r="K45" s="20">
+      <c r="K45" s="14">
         <v>0.20030000000000001</v>
       </c>
-      <c r="L45" s="20">
+      <c r="L45" s="14">
         <v>79.966499999999996</v>
       </c>
-      <c r="M45" s="20" t="s">
+      <c r="M45" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N45" s="20">
+      <c r="N45" s="14">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O45" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="45"/>
-      <c r="B46" s="20">
+      <c r="O45" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P45" s="61"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" s="39"/>
+      <c r="B46" s="14">
         <v>6</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D46" s="20">
+      <c r="D46" s="14">
         <v>0.97089999999999999</v>
       </c>
-      <c r="E46" s="20">
+      <c r="E46" s="14">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F46" s="20">
+      <c r="F46" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G46" s="20">
+      <c r="G46" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I46" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J46" s="20">
+      <c r="I46" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J46" s="14">
         <v>-0.42680000000000001</v>
       </c>
-      <c r="K46" s="20">
+      <c r="K46" s="14">
         <v>0.67459999999999998</v>
       </c>
-      <c r="L46" s="20">
+      <c r="L46" s="14">
         <v>32.544400000000003</v>
       </c>
-      <c r="M46" s="20" t="s">
+      <c r="M46" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N46" s="20">
+      <c r="N46" s="14">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="O46" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="45"/>
-      <c r="B47" s="20">
+      <c r="O46" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P46" s="61"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47" s="39"/>
+      <c r="B47" s="14">
         <v>7</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D47" s="20">
+      <c r="D47" s="14">
         <v>0.97250000000000003</v>
       </c>
-      <c r="E47" s="20">
+      <c r="E47" s="14">
         <v>1E-3</v>
       </c>
-      <c r="F47" s="20">
+      <c r="F47" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G47" s="20">
+      <c r="G47" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H47" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I47" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J47" s="20">
+      <c r="H47" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I47" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J47" s="14">
         <v>-3.9144999999999999</v>
       </c>
-      <c r="K47" s="20">
+      <c r="K47" s="14">
         <v>1E-3</v>
       </c>
-      <c r="L47" s="20">
+      <c r="L47" s="14">
         <v>99.898399999999995</v>
       </c>
-      <c r="M47" s="20" t="s">
+      <c r="M47" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N47" s="20">
+      <c r="N47" s="14">
         <v>1.8E-3</v>
       </c>
-      <c r="O47" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="45"/>
-      <c r="B48" s="20">
+      <c r="O47" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P47" s="61" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" s="39"/>
+      <c r="B48" s="14">
         <v>8</v>
       </c>
-      <c r="C48" s="20" t="s">
+      <c r="C48" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D48" s="20">
+      <c r="D48" s="14">
         <v>0.97209999999999996</v>
       </c>
-      <c r="E48" s="20">
+      <c r="E48" s="14">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="F48" s="20">
+      <c r="F48" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G48" s="20">
+      <c r="G48" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H48" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I48" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J48" s="20">
+      <c r="H48" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I48" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J48" s="14">
         <v>-3.5063</v>
       </c>
-      <c r="K48" s="20">
+      <c r="K48" s="14">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="L48" s="20">
+      <c r="L48" s="14">
         <v>99.747900000000001</v>
       </c>
-      <c r="M48" s="20" t="s">
+      <c r="M48" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N48" s="20">
+      <c r="N48" s="14">
         <v>1.4E-3</v>
       </c>
-      <c r="O48" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="45"/>
-      <c r="B49" s="20">
+      <c r="O48" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P48" s="61"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A49" s="39"/>
+      <c r="B49" s="14">
         <v>9</v>
       </c>
-      <c r="C49" s="20" t="s">
+      <c r="C49" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D49" s="20">
+      <c r="D49" s="14">
         <v>0.9718</v>
       </c>
-      <c r="E49" s="20">
+      <c r="E49" s="14">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="F49" s="20">
+      <c r="F49" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G49" s="20">
+      <c r="G49" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H49" s="21" t="s">
+      <c r="H49" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I49" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J49" s="20">
+      <c r="I49" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J49" s="14">
         <v>-2.2578999999999998</v>
       </c>
-      <c r="K49" s="20">
+      <c r="K49" s="14">
         <v>3.6600000000000001E-2</v>
       </c>
-      <c r="L49" s="20">
+      <c r="L49" s="14">
         <v>96.339100000000002</v>
       </c>
-      <c r="M49" s="20" t="s">
+      <c r="M49" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N49" s="20">
+      <c r="N49" s="14">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="O49" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="45"/>
-      <c r="B50" s="20">
+      <c r="O49" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P49" s="61"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A50" s="39"/>
+      <c r="B50" s="14">
         <v>10</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C50" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D50" s="20">
+      <c r="D50" s="14">
         <v>0.97250000000000003</v>
       </c>
-      <c r="E50" s="20">
+      <c r="E50" s="14">
         <v>1E-3</v>
       </c>
-      <c r="F50" s="20">
+      <c r="F50" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G50" s="20">
+      <c r="G50" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H50" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I50" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J50" s="20">
+      <c r="H50" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I50" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J50" s="14">
         <v>-3.9502000000000002</v>
       </c>
-      <c r="K50" s="20">
+      <c r="K50" s="14">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="L50" s="20">
+      <c r="L50" s="14">
         <v>99.906199999999998</v>
       </c>
-      <c r="M50" s="20" t="s">
+      <c r="M50" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N50" s="20">
+      <c r="N50" s="14">
         <v>1.8E-3</v>
       </c>
-      <c r="O50" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="45"/>
-      <c r="B51" s="20">
+      <c r="O50" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P50" s="61"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A51" s="39"/>
+      <c r="B51" s="14">
         <v>11</v>
       </c>
-      <c r="C51" s="20" t="s">
+      <c r="C51" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D51" s="20">
+      <c r="D51" s="14">
         <v>0.97270000000000001</v>
       </c>
-      <c r="E51" s="20">
+      <c r="E51" s="14">
         <v>1.4E-3</v>
       </c>
-      <c r="F51" s="20">
+      <c r="F51" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G51" s="20">
+      <c r="G51" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H51" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I51" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J51" s="20">
+      <c r="H51" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I51" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J51" s="14">
         <v>-3.8056000000000001</v>
       </c>
-      <c r="K51" s="20">
+      <c r="K51" s="14">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="L51" s="20">
+      <c r="L51" s="14">
         <v>99.870500000000007</v>
       </c>
-      <c r="M51" s="20" t="s">
+      <c r="M51" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N51" s="20">
+      <c r="N51" s="14">
         <v>2E-3</v>
       </c>
-      <c r="O51" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="45"/>
-      <c r="B52" s="20">
+      <c r="O51" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P51" s="61"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52" s="39"/>
+      <c r="B52" s="14">
         <v>12</v>
       </c>
-      <c r="C52" s="20" t="s">
+      <c r="C52" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D52" s="20">
+      <c r="D52" s="14">
         <v>0.97299999999999998</v>
       </c>
-      <c r="E52" s="20">
+      <c r="E52" s="14">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="F52" s="20">
+      <c r="F52" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G52" s="20">
+      <c r="G52" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H52" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I52" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J52" s="20">
+      <c r="H52" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I52" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J52" s="14">
         <v>-5.4046000000000003</v>
       </c>
-      <c r="K52" s="20">
+      <c r="K52" s="14">
         <v>0</v>
       </c>
-      <c r="L52" s="20">
+      <c r="L52" s="14">
         <v>99.996099999999998</v>
       </c>
-      <c r="M52" s="20" t="s">
+      <c r="M52" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N52" s="20">
+      <c r="N52" s="14">
         <v>2.3E-3</v>
       </c>
-      <c r="O52" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="45"/>
-      <c r="B53" s="20">
+      <c r="O52" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P52" s="61"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53" s="39"/>
+      <c r="B53" s="14">
         <v>13</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D53" s="20">
+      <c r="D53" s="14">
         <v>0.97230000000000005</v>
       </c>
-      <c r="E53" s="20">
+      <c r="E53" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="F53" s="20">
+      <c r="F53" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G53" s="20">
+      <c r="G53" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H53" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I53" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J53" s="20">
+      <c r="H53" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I53" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J53" s="14">
         <v>-3.9950000000000001</v>
       </c>
-      <c r="K53" s="20">
+      <c r="K53" s="14">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="L53" s="20">
+      <c r="L53" s="14">
         <v>99.915099999999995</v>
       </c>
-      <c r="M53" s="20" t="s">
+      <c r="M53" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N53" s="20">
+      <c r="N53" s="14">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="O53" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="45"/>
-      <c r="B54" s="20">
+      <c r="O53" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P53" s="61"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A54" s="39"/>
+      <c r="B54" s="14">
         <v>14</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D54" s="20">
+      <c r="D54" s="14">
         <v>0.97250000000000003</v>
       </c>
-      <c r="E54" s="20">
+      <c r="E54" s="14">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="F54" s="20">
+      <c r="F54" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G54" s="20">
+      <c r="G54" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H54" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I54" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J54" s="20">
+      <c r="H54" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I54" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J54" s="14">
         <v>-3.4491000000000001</v>
       </c>
-      <c r="K54" s="20">
+      <c r="K54" s="14">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="L54" s="20">
+      <c r="L54" s="14">
         <v>99.713800000000006</v>
       </c>
-      <c r="M54" s="20" t="s">
+      <c r="M54" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N54" s="20">
+      <c r="N54" s="14">
         <v>1.8E-3</v>
       </c>
-      <c r="O54" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="45"/>
-      <c r="B55" s="20">
+      <c r="O54" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P54" s="61"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A55" s="39"/>
+      <c r="B55" s="14">
         <v>15</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D55" s="20">
+      <c r="D55" s="14">
         <v>0.97189999999999999</v>
       </c>
-      <c r="E55" s="20">
+      <c r="E55" s="14">
         <v>1.9E-3</v>
       </c>
-      <c r="F55" s="20">
+      <c r="F55" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G55" s="20">
+      <c r="G55" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H55" s="21" t="s">
+      <c r="H55" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I55" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J55" s="20">
+      <c r="I55" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J55" s="14">
         <v>-1.8017000000000001</v>
       </c>
-      <c r="K55" s="20">
+      <c r="K55" s="14">
         <v>8.8400000000000006E-2</v>
       </c>
-      <c r="L55" s="20">
+      <c r="L55" s="14">
         <v>91.162999999999997</v>
       </c>
-      <c r="M55" s="20" t="s">
+      <c r="M55" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N55" s="20">
+      <c r="N55" s="14">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="O55" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="45"/>
-      <c r="B56" s="20">
+      <c r="O55" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P55" s="61"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A56" s="39"/>
+      <c r="B56" s="14">
         <v>16</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="C56" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D56" s="20">
+      <c r="D56" s="14">
         <v>0.97140000000000004</v>
       </c>
-      <c r="E56" s="20">
+      <c r="E56" s="14">
         <v>1.9E-3</v>
       </c>
-      <c r="F56" s="20">
+      <c r="F56" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G56" s="20">
+      <c r="G56" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H56" s="21" t="s">
+      <c r="H56" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I56" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J56" s="20">
+      <c r="I56" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J56" s="14">
         <v>-1.0462</v>
       </c>
-      <c r="K56" s="20">
+      <c r="K56" s="14">
         <v>0.30930000000000002</v>
       </c>
-      <c r="L56" s="20">
+      <c r="L56" s="14">
         <v>69.069100000000006</v>
       </c>
-      <c r="M56" s="20" t="s">
+      <c r="M56" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N56" s="20">
+      <c r="N56" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="O56" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="45"/>
-      <c r="B57" s="20">
-        <v>17</v>
-      </c>
-      <c r="C57" s="20" t="s">
+      <c r="O56" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P56" s="61" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A57" s="39"/>
+      <c r="B57" s="14">
+        <v>17</v>
+      </c>
+      <c r="C57" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="20">
+      <c r="D57" s="14">
         <v>0.97140000000000004</v>
       </c>
-      <c r="E57" s="20">
+      <c r="E57" s="14">
         <v>1E-3</v>
       </c>
-      <c r="F57" s="20">
+      <c r="F57" s="14">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G57" s="20">
+      <c r="G57" s="14">
         <v>1E-3</v>
       </c>
-      <c r="H57" s="21" t="s">
+      <c r="H57" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I57" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J57" s="20">
+      <c r="I57" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="J57" s="14">
         <v>-1.5361</v>
       </c>
-      <c r="K57" s="20">
+      <c r="K57" s="14">
         <v>0.1419</v>
       </c>
-      <c r="L57" s="20">
+      <c r="L57" s="14">
         <v>85.809299999999993</v>
       </c>
-      <c r="M57" s="20" t="s">
+      <c r="M57" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N57" s="20">
+      <c r="N57" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="O57" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="46"/>
-      <c r="B58" s="26">
+      <c r="O57" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P57" s="61"/>
+    </row>
+    <row r="58" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="40"/>
+      <c r="B58" s="18">
         <v>18</v>
       </c>
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D58" s="26">
+      <c r="D58" s="18">
         <v>0.97030000000000005</v>
       </c>
-      <c r="E58" s="26">
+      <c r="E58" s="18">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="F58" s="26">
+      <c r="F58" s="18">
         <v>0.97070000000000001</v>
       </c>
-      <c r="G58" s="26">
+      <c r="G58" s="18">
         <v>1E-3</v>
       </c>
-      <c r="H58" s="27" t="s">
+      <c r="H58" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="I58" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="J58" s="26">
+      <c r="I58" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="J58" s="18">
         <v>1.0148999999999999</v>
       </c>
-      <c r="K58" s="26">
+      <c r="K58" s="18">
         <v>0.3236</v>
       </c>
-      <c r="L58" s="26">
+      <c r="L58" s="18">
         <v>67.637799999999999</v>
       </c>
-      <c r="M58" s="26" t="s">
+      <c r="M58" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="N58" s="26">
+      <c r="N58" s="18">
         <v>-4.0000000000000002E-4</v>
       </c>
-      <c r="O58" s="28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A59" s="47" t="s">
+      <c r="O58" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="P58" s="62"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A59" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="B59" s="31">
+      <c r="B59" s="22">
         <v>0</v>
       </c>
-      <c r="C59" s="31" t="s">
+      <c r="C59" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="31">
+      <c r="D59" s="22">
         <v>0.93659999999999999</v>
       </c>
-      <c r="E59" s="31">
+      <c r="E59" s="22">
         <v>1.9E-3</v>
       </c>
-      <c r="F59" s="31">
+      <c r="F59" s="22">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G59" s="31">
+      <c r="G59" s="22">
         <v>1.8E-3</v>
       </c>
-      <c r="H59" s="32" t="s">
+      <c r="H59" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="I59" s="31">
-        <v>0.03</v>
-      </c>
-      <c r="J59" s="31">
+      <c r="I59" s="22">
+        <v>0.03</v>
+      </c>
+      <c r="J59" s="22">
         <v>-1.2478</v>
       </c>
-      <c r="K59" s="31">
+      <c r="K59" s="22">
         <v>0.2281</v>
       </c>
-      <c r="L59" s="31">
+      <c r="L59" s="22">
         <v>77.190399999999997</v>
       </c>
-      <c r="M59" s="31" t="s">
+      <c r="M59" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="N59" s="31">
+      <c r="N59" s="22">
         <v>1E-3</v>
       </c>
-      <c r="O59" s="33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A60" s="48"/>
-      <c r="B60" s="29">
+      <c r="O59" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="P59" s="63" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A60" s="42"/>
+      <c r="B60" s="20">
         <v>1</v>
       </c>
-      <c r="C60" s="29" t="s">
+      <c r="C60" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D60" s="29">
+      <c r="D60" s="20">
         <v>0.93730000000000002</v>
       </c>
-      <c r="E60" s="29">
+      <c r="E60" s="20">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="F60" s="29">
+      <c r="F60" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G60" s="29">
+      <c r="G60" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H60" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I60" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J60" s="29">
+      <c r="H60" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I60" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J60" s="20">
         <v>-2.3641000000000001</v>
       </c>
-      <c r="K60" s="29">
+      <c r="K60" s="20">
         <v>2.9499999999999998E-2</v>
       </c>
-      <c r="L60" s="29">
+      <c r="L60" s="20">
         <v>97.048100000000005</v>
       </c>
-      <c r="M60" s="29" t="s">
+      <c r="M60" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="N60" s="29">
+      <c r="N60" s="20">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="O60" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A61" s="48"/>
-      <c r="B61" s="50">
+      <c r="O60" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P60" s="61"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A61" s="42"/>
+      <c r="B61" s="26">
         <v>2</v>
       </c>
-      <c r="C61" s="50" t="s">
+      <c r="C61" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D61" s="50">
+      <c r="D61" s="26">
         <v>0.93830000000000002</v>
       </c>
-      <c r="E61" s="50">
+      <c r="E61" s="26">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="F61" s="50">
+      <c r="F61" s="26">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G61" s="50">
+      <c r="G61" s="26">
         <v>1.8E-3</v>
       </c>
-      <c r="H61" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="I61" s="50">
-        <v>0.03</v>
-      </c>
-      <c r="J61" s="50">
+      <c r="H61" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I61" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="J61" s="26">
         <v>-3.8574000000000002</v>
       </c>
-      <c r="K61" s="50">
+      <c r="K61" s="26">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="L61" s="50">
+      <c r="L61" s="26">
         <v>99.884600000000006</v>
       </c>
-      <c r="M61" s="50" t="s">
+      <c r="M61" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="N61" s="50">
+      <c r="N61" s="26">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="O61" s="52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A62" s="48"/>
-      <c r="B62" s="29">
+      <c r="O61" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="P61" s="61"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A62" s="42"/>
+      <c r="B62" s="20">
         <v>3</v>
       </c>
-      <c r="C62" s="29" t="s">
+      <c r="C62" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="29">
+      <c r="D62" s="20">
         <v>0.9294</v>
       </c>
-      <c r="E62" s="29">
+      <c r="E62" s="20">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="F62" s="29">
+      <c r="F62" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G62" s="29">
+      <c r="G62" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H62" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I62" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J62" s="29">
+      <c r="H62" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I62" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J62" s="20">
         <v>5.3971999999999998</v>
       </c>
-      <c r="K62" s="29">
+      <c r="K62" s="20">
         <v>0</v>
       </c>
-      <c r="L62" s="29">
+      <c r="L62" s="20">
         <v>99.995999999999995</v>
       </c>
-      <c r="M62" s="29" t="s">
+      <c r="M62" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N62" s="29">
+      <c r="N62" s="20">
         <v>-6.1999999999999998E-3</v>
       </c>
-      <c r="O62" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A63" s="48"/>
-      <c r="B63" s="29">
+      <c r="O62" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P62" s="61" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A63" s="42"/>
+      <c r="B63" s="20">
         <v>4</v>
       </c>
-      <c r="C63" s="29" t="s">
+      <c r="C63" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D63" s="29">
+      <c r="D63" s="20">
         <v>0.93430000000000002</v>
       </c>
-      <c r="E63" s="29">
+      <c r="E63" s="20">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="F63" s="29">
+      <c r="F63" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G63" s="29">
+      <c r="G63" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H63" s="30" t="s">
+      <c r="H63" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I63" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J63" s="29">
+      <c r="I63" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J63" s="20">
         <v>1.4769000000000001</v>
       </c>
-      <c r="K63" s="29">
+      <c r="K63" s="20">
         <v>0.157</v>
       </c>
-      <c r="L63" s="29">
+      <c r="L63" s="20">
         <v>84.301000000000002</v>
       </c>
-      <c r="M63" s="29" t="s">
+      <c r="M63" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N63" s="29">
+      <c r="N63" s="20">
         <v>-1.2999999999999999E-3</v>
       </c>
-      <c r="O63" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="48"/>
-      <c r="B64" s="29">
+      <c r="O63" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P63" s="61"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A64" s="42"/>
+      <c r="B64" s="20">
         <v>5</v>
       </c>
-      <c r="C64" s="29" t="s">
+      <c r="C64" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D64" s="29">
+      <c r="D64" s="20">
         <v>0.9234</v>
       </c>
-      <c r="E64" s="29">
+      <c r="E64" s="20">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="F64" s="29">
+      <c r="F64" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G64" s="29">
+      <c r="G64" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H64" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I64" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J64" s="29">
+      <c r="H64" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I64" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J64" s="20">
         <v>9.0916999999999994</v>
       </c>
-      <c r="K64" s="29">
+      <c r="K64" s="20">
         <v>0</v>
       </c>
-      <c r="L64" s="29">
+      <c r="L64" s="20">
         <v>99.999899999999997</v>
       </c>
-      <c r="M64" s="29" t="s">
+      <c r="M64" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N64" s="29">
+      <c r="N64" s="20">
         <v>-1.2200000000000001E-2</v>
       </c>
-      <c r="O64" s="34" t="s">
+      <c r="O64" s="45" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="48"/>
-      <c r="B65" s="29">
+      <c r="P64" s="61"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A65" s="42"/>
+      <c r="B65" s="20">
         <v>6</v>
       </c>
-      <c r="C65" s="29" t="s">
+      <c r="C65" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D65" s="29">
+      <c r="D65" s="20">
         <v>0.89349999999999996</v>
       </c>
-      <c r="E65" s="29">
+      <c r="E65" s="20">
         <v>1.5E-3</v>
       </c>
-      <c r="F65" s="29">
+      <c r="F65" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G65" s="29">
+      <c r="G65" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H65" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I65" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J65" s="29">
+      <c r="H65" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I65" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J65" s="20">
         <v>57.100200000000001</v>
       </c>
-      <c r="K65" s="29">
+      <c r="K65" s="20">
         <v>0</v>
       </c>
-      <c r="L65" s="29">
+      <c r="L65" s="20">
         <v>100</v>
       </c>
-      <c r="M65" s="29" t="s">
+      <c r="M65" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N65" s="29">
+      <c r="N65" s="20">
         <v>-4.2099999999999999E-2</v>
       </c>
-      <c r="O65" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="48"/>
-      <c r="B66" s="29">
+      <c r="O65" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P65" s="61"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A66" s="42"/>
+      <c r="B66" s="20">
         <v>7</v>
       </c>
-      <c r="C66" s="29" t="s">
+      <c r="C66" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D66" s="29">
+      <c r="D66" s="20">
         <v>0.93799999999999994</v>
       </c>
-      <c r="E66" s="29">
+      <c r="E66" s="20">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="F66" s="29">
+      <c r="F66" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G66" s="29">
+      <c r="G66" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H66" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I66" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J66" s="29">
+      <c r="H66" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I66" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J66" s="20">
         <v>-3.8033999999999999</v>
       </c>
-      <c r="K66" s="29">
+      <c r="K66" s="20">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="L66" s="29">
+      <c r="L66" s="20">
         <v>99.869900000000001</v>
       </c>
-      <c r="M66" s="29" t="s">
+      <c r="M66" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="N66" s="29">
+      <c r="N66" s="20">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="O66" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="48"/>
-      <c r="B67" s="29">
+      <c r="O66" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P66" s="61" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A67" s="42"/>
+      <c r="B67" s="20">
         <v>8</v>
       </c>
-      <c r="C67" s="29" t="s">
+      <c r="C67" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D67" s="29">
+      <c r="D67" s="20">
         <v>0.93730000000000002</v>
       </c>
-      <c r="E67" s="29">
+      <c r="E67" s="20">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="F67" s="29">
+      <c r="F67" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G67" s="29">
+      <c r="G67" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H67" s="30" t="s">
+      <c r="H67" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I67" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J67" s="29">
+      <c r="I67" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J67" s="20">
         <v>-2.2919</v>
       </c>
-      <c r="K67" s="29">
+      <c r="K67" s="20">
         <v>3.4200000000000001E-2</v>
       </c>
-      <c r="L67" s="29">
+      <c r="L67" s="20">
         <v>96.581800000000001</v>
       </c>
-      <c r="M67" s="29" t="s">
+      <c r="M67" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="N67" s="29">
+      <c r="N67" s="20">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="O67" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="48"/>
-      <c r="B68" s="29">
+      <c r="O67" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P67" s="61"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A68" s="42"/>
+      <c r="B68" s="20">
         <v>9</v>
       </c>
-      <c r="C68" s="29" t="s">
+      <c r="C68" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D68" s="29">
+      <c r="D68" s="20">
         <v>0.93679999999999997</v>
       </c>
-      <c r="E68" s="29">
+      <c r="E68" s="20">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="F68" s="29">
+      <c r="F68" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G68" s="29">
+      <c r="G68" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H68" s="30" t="s">
+      <c r="H68" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I68" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J68" s="29">
+      <c r="I68" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J68" s="20">
         <v>-1.7094</v>
       </c>
-      <c r="K68" s="29">
+      <c r="K68" s="20">
         <v>0.1046</v>
       </c>
-      <c r="L68" s="29">
+      <c r="L68" s="20">
         <v>89.543300000000002</v>
       </c>
-      <c r="M68" s="29" t="s">
+      <c r="M68" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="N68" s="29">
+      <c r="N68" s="20">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="O68" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="48"/>
-      <c r="B69" s="29">
+      <c r="O68" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P68" s="61"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A69" s="42"/>
+      <c r="B69" s="20">
         <v>10</v>
       </c>
-      <c r="C69" s="29" t="s">
+      <c r="C69" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D69" s="29">
+      <c r="D69" s="20">
         <v>0.93710000000000004</v>
       </c>
-      <c r="E69" s="29">
+      <c r="E69" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="F69" s="29">
+      <c r="F69" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G69" s="29">
+      <c r="G69" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H69" s="30" t="s">
+      <c r="H69" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I69" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J69" s="29">
+      <c r="I69" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J69" s="20">
         <v>-1.8758999999999999</v>
       </c>
-      <c r="K69" s="29">
+      <c r="K69" s="20">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="L69" s="29">
+      <c r="L69" s="20">
         <v>92.302199999999999</v>
       </c>
-      <c r="M69" s="29" t="s">
+      <c r="M69" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="N69" s="29">
+      <c r="N69" s="20">
         <v>1.5E-3</v>
       </c>
-      <c r="O69" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="48"/>
-      <c r="B70" s="29">
+      <c r="O69" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P69" s="61"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A70" s="42"/>
+      <c r="B70" s="20">
         <v>11</v>
       </c>
-      <c r="C70" s="29" t="s">
+      <c r="C70" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D70" s="29">
+      <c r="D70" s="20">
         <v>0.93720000000000003</v>
       </c>
-      <c r="E70" s="29">
+      <c r="E70" s="20">
         <v>1.9E-3</v>
       </c>
-      <c r="F70" s="29">
+      <c r="F70" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G70" s="29">
+      <c r="G70" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H70" s="30" t="s">
+      <c r="H70" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I70" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J70" s="29">
+      <c r="I70" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J70" s="20">
         <v>-1.9417</v>
       </c>
-      <c r="K70" s="29">
+      <c r="K70" s="20">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="L70" s="29">
+      <c r="L70" s="20">
         <v>93.201300000000003</v>
       </c>
-      <c r="M70" s="29" t="s">
+      <c r="M70" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="N70" s="29">
+      <c r="N70" s="20">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="O70" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A71" s="48"/>
-      <c r="B71" s="29">
+      <c r="O70" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P70" s="61"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A71" s="42"/>
+      <c r="B71" s="20">
         <v>12</v>
       </c>
-      <c r="C71" s="29" t="s">
+      <c r="C71" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D71" s="29">
+      <c r="D71" s="20">
         <v>0.93420000000000003</v>
       </c>
-      <c r="E71" s="29">
+      <c r="E71" s="20">
         <v>1.9E-3</v>
       </c>
-      <c r="F71" s="29">
+      <c r="F71" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G71" s="29">
+      <c r="G71" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H71" s="30" t="s">
+      <c r="H71" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I71" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J71" s="29">
+      <c r="I71" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J71" s="20">
         <v>1.7462</v>
       </c>
-      <c r="K71" s="29">
+      <c r="K71" s="20">
         <v>9.7799999999999998E-2</v>
       </c>
-      <c r="L71" s="29">
+      <c r="L71" s="20">
         <v>90.217500000000001</v>
       </c>
-      <c r="M71" s="29" t="s">
+      <c r="M71" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N71" s="29">
+      <c r="N71" s="20">
         <v>-1.4E-3</v>
       </c>
-      <c r="O71" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="48"/>
-      <c r="B72" s="29">
+      <c r="O71" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P71" s="61"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A72" s="42"/>
+      <c r="B72" s="20">
         <v>13</v>
       </c>
-      <c r="C72" s="29" t="s">
+      <c r="C72" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D72" s="29">
+      <c r="D72" s="20">
         <v>0.93400000000000005</v>
       </c>
-      <c r="E72" s="29">
+      <c r="E72" s="20">
         <v>3.3E-3</v>
       </c>
-      <c r="F72" s="29">
+      <c r="F72" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G72" s="29">
+      <c r="G72" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H72" s="30" t="s">
+      <c r="H72" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I72" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J72" s="29">
+      <c r="I72" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J72" s="20">
         <v>1.3854</v>
       </c>
-      <c r="K72" s="29">
+      <c r="K72" s="20">
         <v>0.18279999999999999</v>
       </c>
-      <c r="L72" s="29">
+      <c r="L72" s="20">
         <v>81.715400000000002</v>
       </c>
-      <c r="M72" s="29" t="s">
+      <c r="M72" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N72" s="29">
+      <c r="N72" s="20">
         <v>-1.6000000000000001E-3</v>
       </c>
-      <c r="O72" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A73" s="48"/>
-      <c r="B73" s="29">
+      <c r="O72" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P72" s="61"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A73" s="42"/>
+      <c r="B73" s="20">
         <v>14</v>
       </c>
-      <c r="C73" s="29" t="s">
+      <c r="C73" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D73" s="29">
+      <c r="D73" s="20">
         <v>0.93269999999999997</v>
       </c>
-      <c r="E73" s="29">
+      <c r="E73" s="20">
         <v>4.1000000000000003E-3</v>
       </c>
-      <c r="F73" s="29">
+      <c r="F73" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G73" s="29">
+      <c r="G73" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H73" s="30" t="s">
+      <c r="H73" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I73" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J73" s="29">
+      <c r="I73" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J73" s="20">
         <v>2.0051000000000001</v>
       </c>
-      <c r="K73" s="29">
+      <c r="K73" s="20">
         <v>6.7400000000000002E-2</v>
       </c>
-      <c r="L73" s="29">
+      <c r="L73" s="20">
         <v>93.255499999999998</v>
       </c>
-      <c r="M73" s="29" t="s">
+      <c r="M73" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N73" s="29">
+      <c r="N73" s="20">
         <v>-2.8999999999999998E-3</v>
       </c>
-      <c r="O73" s="34" t="s">
+      <c r="O73" s="45" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A74" s="48"/>
-      <c r="B74" s="29">
+      <c r="P73" s="61"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A74" s="42"/>
+      <c r="B74" s="20">
         <v>15</v>
       </c>
-      <c r="C74" s="29" t="s">
+      <c r="C74" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D74" s="29">
+      <c r="D74" s="20">
         <v>0.92600000000000005</v>
       </c>
-      <c r="E74" s="29">
+      <c r="E74" s="20">
         <v>3.3E-3</v>
       </c>
-      <c r="F74" s="29">
+      <c r="F74" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G74" s="29">
+      <c r="G74" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H74" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I74" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J74" s="29">
+      <c r="H74" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I74" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J74" s="20">
         <v>8.1428999999999991</v>
       </c>
-      <c r="K74" s="29">
+      <c r="K74" s="20">
         <v>0</v>
       </c>
-      <c r="L74" s="29">
+      <c r="L74" s="20">
         <v>100</v>
       </c>
-      <c r="M74" s="29" t="s">
+      <c r="M74" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N74" s="29">
+      <c r="N74" s="20">
         <v>-9.5999999999999992E-3</v>
       </c>
-      <c r="O74" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A75" s="48"/>
-      <c r="B75" s="29">
+      <c r="O74" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P74" s="61"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A75" s="42"/>
+      <c r="B75" s="20">
         <v>16</v>
       </c>
-      <c r="C75" s="29" t="s">
+      <c r="C75" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D75" s="29">
+      <c r="D75" s="20">
         <v>0.92369999999999997</v>
       </c>
-      <c r="E75" s="29">
+      <c r="E75" s="20">
         <v>6.1000000000000004E-3</v>
       </c>
-      <c r="F75" s="29">
+      <c r="F75" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G75" s="29">
+      <c r="G75" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H75" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I75" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J75" s="29">
+      <c r="H75" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I75" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J75" s="20">
         <v>5.9676999999999998</v>
       </c>
-      <c r="K75" s="29">
+      <c r="K75" s="20">
         <v>1E-4</v>
       </c>
-      <c r="L75" s="29">
+      <c r="L75" s="20">
         <v>99.989000000000004</v>
       </c>
-      <c r="M75" s="29" t="s">
+      <c r="M75" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N75" s="29">
+      <c r="N75" s="20">
         <v>-1.1900000000000001E-2</v>
       </c>
-      <c r="O75" s="34" t="s">
+      <c r="O75" s="45" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A76" s="48"/>
-      <c r="B76" s="29">
-        <v>17</v>
-      </c>
-      <c r="C76" s="29" t="s">
+      <c r="P75" s="61" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A76" s="42"/>
+      <c r="B76" s="20">
+        <v>17</v>
+      </c>
+      <c r="C76" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D76" s="29">
+      <c r="D76" s="20">
         <v>0.9375</v>
       </c>
-      <c r="E76" s="29">
+      <c r="E76" s="20">
         <v>2E-3</v>
       </c>
-      <c r="F76" s="29">
+      <c r="F76" s="20">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G76" s="29">
+      <c r="G76" s="20">
         <v>1.8E-3</v>
       </c>
-      <c r="H76" s="30" t="s">
+      <c r="H76" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I76" s="29">
-        <v>0.03</v>
-      </c>
-      <c r="J76" s="29">
+      <c r="I76" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="J76" s="20">
         <v>-2.2121</v>
       </c>
-      <c r="K76" s="29">
+      <c r="K76" s="20">
         <v>4.0099999999999997E-2</v>
       </c>
-      <c r="L76" s="29">
+      <c r="L76" s="20">
         <v>95.986999999999995</v>
       </c>
-      <c r="M76" s="29" t="s">
+      <c r="M76" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="N76" s="29">
+      <c r="N76" s="20">
         <v>1.9E-3</v>
       </c>
-      <c r="O76" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="49"/>
-      <c r="B77" s="35">
+      <c r="O76" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P76" s="61"/>
+    </row>
+    <row r="77" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="43"/>
+      <c r="B77" s="24">
         <v>18</v>
       </c>
-      <c r="C77" s="35" t="s">
+      <c r="C77" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D77" s="35">
+      <c r="D77" s="24">
         <v>0.93740000000000001</v>
       </c>
-      <c r="E77" s="35">
+      <c r="E77" s="24">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="F77" s="35">
+      <c r="F77" s="24">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G77" s="35">
+      <c r="G77" s="24">
         <v>1.8E-3</v>
       </c>
-      <c r="H77" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="I77" s="35">
-        <v>0.03</v>
-      </c>
-      <c r="J77" s="35">
+      <c r="H77" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="I77" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="J77" s="24">
         <v>-2.7583000000000002</v>
       </c>
-      <c r="K77" s="35">
+      <c r="K77" s="24">
         <v>1.29E-2</v>
       </c>
-      <c r="L77" s="35">
+      <c r="L77" s="24">
         <v>98.706000000000003</v>
       </c>
-      <c r="M77" s="35" t="s">
+      <c r="M77" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="N77" s="35">
+      <c r="N77" s="24">
         <v>1.8E-3</v>
       </c>
-      <c r="O77" s="37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
+      <c r="O77" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="P77" s="62"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="20">
+    <mergeCell ref="P59:P61"/>
+    <mergeCell ref="P62:P65"/>
+    <mergeCell ref="P66:P74"/>
+    <mergeCell ref="P75:P77"/>
     <mergeCell ref="A2:A20"/>
     <mergeCell ref="A21:A39"/>
     <mergeCell ref="A40:A58"/>
     <mergeCell ref="A59:A77"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="P5:P8"/>
+    <mergeCell ref="P9:P17"/>
+    <mergeCell ref="P18:P20"/>
+    <mergeCell ref="P21:P23"/>
+    <mergeCell ref="P24:P27"/>
+    <mergeCell ref="P28:P36"/>
+    <mergeCell ref="P37:P39"/>
+    <mergeCell ref="P40:P42"/>
+    <mergeCell ref="P43:P46"/>
+    <mergeCell ref="P47:P55"/>
+    <mergeCell ref="P56:P58"/>
   </mergeCells>
   <conditionalFormatting sqref="H2:H77">
-    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="Reject H0">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Reject H0">
       <formula>NOT(ISERROR(SEARCH("Reject H0",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Fail to reject H0">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Fail to reject H0">
       <formula>NOT(ISERROR(SEARCH("Fail to reject H0",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L77">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O77">
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="True">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="True">
       <formula>NOT(ISERROR(SEARCH("True",O2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="False">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="False">
       <formula>NOT(ISERROR(SEARCH("False",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M77">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Original">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Original">
       <formula>NOT(ISERROR(SEARCH("Original",M2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Experiment">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Experiment">
       <formula>NOT(ISERROR(SEARCH("Experiment",M2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>